<commit_message>
Performance test results updated
</commit_message>
<xml_diff>
--- a/performance_test/results.xlsx
+++ b/performance_test/results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matyi/Development/GitHub/TURMU/performance_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matyi/PycharmProjects/TURMU/performance_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51BEB7D0-FE71-2747-96B5-7C52080F0E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A058109B-9EE8-304F-BE36-5AF975B7CFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="11420" windowWidth="28240" windowHeight="17240" xr2:uid="{73779BE7-D483-A54E-B212-8D7835BC9426}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="28800" windowHeight="15820" xr2:uid="{73779BE7-D483-A54E-B212-8D7835BC9426}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t>T_(alpha)</t>
   </si>
@@ -50,47 +49,34 @@
     <t>Dt_on (s)</t>
   </si>
   <si>
-    <t>sigma</t>
+    <t>AVG</t>
   </si>
   <si>
-    <t>-2.871197204438977</t>
+    <t>VAR</t>
   </si>
   <si>
-    <t>-2.871198056243275</t>
-  </si>
-  <si>
-    <t>-2.8711836478018453</t>
-  </si>
-  <si>
-    <t>-2.871181198118343</t>
-  </si>
-  <si>
-    <t>-2.8711984315720294</t>
-  </si>
-  <si>
-    <t>-2.8712039209382327</t>
-  </si>
-  <si>
-    <t>-2.8712006882970784</t>
-  </si>
-  <si>
-    <t>-2.871191329582031</t>
-  </si>
-  <si>
-    <t>-2.871201072925966</t>
-  </si>
-  <si>
-    <t>-2.8711958881977075</t>
+    <t>Delta_sum (m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -117,11 +103,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -137,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -433,18 +422,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587BA784-E65A-9145-8D36-E69A42435349}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,106 +448,876 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>19.40494</v>
+        <v>20.315059000000002</v>
       </c>
       <c r="C2">
-        <v>22.263566000000001</v>
+        <v>23.502621999999999</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D11" si="0">C2-B2</f>
-        <v>2.858626000000001</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.1875629999999973</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4.42881400697933E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>43.911541</v>
+      </c>
+      <c r="C3">
+        <v>47.110430000000001</v>
+      </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.1988890000000012</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>12.257859</v>
+      </c>
+      <c r="C4">
+        <v>15.538581000000001</v>
+      </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.2807220000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>49.762867999999997</v>
+      </c>
+      <c r="C5">
+        <v>53.655543000000002</v>
+      </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.8926750000000041</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>15.715902</v>
+      </c>
+      <c r="C6">
+        <v>19.185701000000002</v>
+      </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.4697990000000019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>28.487493000000001</v>
+      </c>
+      <c r="C7">
+        <v>31.616085999999999</v>
+      </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.1285929999999986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>43.856971999999999</v>
+      </c>
+      <c r="C8">
+        <v>47.001787999999998</v>
+      </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.1448159999999987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>7.5137600000000004</v>
+      </c>
+      <c r="C9">
+        <v>11.087933</v>
+      </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.5741729999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>28.951879000000002</v>
+      </c>
+      <c r="C10">
+        <v>32.572676999999999</v>
+      </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.6207979999999971</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>41.659640000000003</v>
+      </c>
+      <c r="C11">
+        <v>44.78969</v>
+      </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
+        <v>3.1300499999999971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D2:D11)</f>
+        <v>3.3628077999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <f>_xlfn.VAR.S(D2:D11)</f>
+        <v>6.9367993325511759E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>13.23448</v>
+      </c>
+      <c r="C14">
+        <v>16.042031000000001</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D35" si="1">C14-B14</f>
+        <v>2.8075510000000019</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5.3382875592657003E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>15.594817000000001</v>
+      </c>
+      <c r="C15">
+        <v>18.402197999999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2.8073809999999977</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>21.131530999999999</v>
+      </c>
+      <c r="C16">
+        <v>24.231881999999999</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>3.1003509999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>28.613481</v>
+      </c>
+      <c r="C17">
+        <v>31.421876999999999</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2.8083959999999983</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>53.188625999999999</v>
+      </c>
+      <c r="C18">
+        <v>56.035018999999998</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>2.8463929999999991</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>26.491952000000001</v>
+      </c>
+      <c r="C19">
+        <v>29.571508000000001</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>3.0795560000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>32.491357000000001</v>
+      </c>
+      <c r="C20">
+        <v>35.539639000000001</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>3.0482820000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>8.8360660000000006</v>
+      </c>
+      <c r="C21">
+        <v>11.664448999999999</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2.8283829999999988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>31.176252000000002</v>
+      </c>
+      <c r="C22">
+        <v>34.264642000000002</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>3.0883900000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>48.809488000000002</v>
+      </c>
+      <c r="C23">
+        <v>51.674619999999997</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2.8651319999999956</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE(D14:D23)</f>
+        <v>2.9279814999999991</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <f>_xlfn.VAR.S(D14:D23)</f>
+        <v>1.7418272519833522E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>50.250435000000003</v>
+      </c>
+      <c r="C26">
+        <v>52.894571999999997</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>2.6441369999999935</v>
+      </c>
+      <c r="E26" s="3">
+        <v>5.5038466113010503E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>27.677173</v>
+      </c>
+      <c r="C27">
+        <v>30.219062000000001</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>2.5418890000000012</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>53.708658</v>
+      </c>
+      <c r="C28">
+        <v>56.241517000000002</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>2.532859000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>28.979406000000001</v>
+      </c>
+      <c r="C29">
+        <v>31.52355</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>2.5441439999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>4.2843650000000002</v>
+      </c>
+      <c r="C30">
+        <v>6.9162290000000004</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>2.6318640000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>31.294846</v>
+      </c>
+      <c r="C31">
+        <v>33.822612999999997</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>2.5277669999999972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>45.572158000000002</v>
+      </c>
+      <c r="C32">
+        <v>48.102474999999998</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>2.5303169999999966</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>20.695982999999998</v>
+      </c>
+      <c r="C33">
+        <v>23.254574999999999</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>2.5585920000000009</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>32.631995000000003</v>
+      </c>
+      <c r="C34">
+        <v>35.168413000000001</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>2.5364179999999976</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>40.955970999999998</v>
+      </c>
+      <c r="C35">
+        <v>43.731838000000003</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>2.7758670000000052</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <f>AVERAGE(D26:D35)</f>
+        <v>2.5823853999999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <f>_xlfn.VAR.S(D26:D35)</f>
+        <v>6.4027960584890926E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>57.922345999999997</v>
+      </c>
+      <c r="C38">
+        <v>60.418005999999998</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38:D59" si="2">C38-B38</f>
+        <v>2.4956600000000009</v>
+      </c>
+      <c r="E38" s="3">
+        <v>7.3380996437530897E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>25.276748000000001</v>
+      </c>
+      <c r="C39">
+        <v>27.700900000000001</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>2.4241519999999994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>38.678719000000001</v>
+      </c>
+      <c r="C40">
+        <v>40.887625</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>2.2089059999999989</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>51.180663000000003</v>
+      </c>
+      <c r="C41">
+        <v>53.653046000000003</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>2.4723830000000007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>2.1447440000000002</v>
+      </c>
+      <c r="C42">
+        <v>4.3575470000000003</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>2.2128030000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>17.688625999999999</v>
+      </c>
+      <c r="C43">
+        <v>19.921682000000001</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>2.2330560000000013</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>42.363081999999999</v>
+      </c>
+      <c r="C44">
+        <v>44.589042999999997</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>2.2259609999999981</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>55.772663000000001</v>
+      </c>
+      <c r="C45">
+        <v>58.161312000000002</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>2.3886490000000009</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>57.037025999999997</v>
+      </c>
+      <c r="C46">
+        <v>59.418801999999999</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>2.3817760000000021</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>13.744762</v>
+      </c>
+      <c r="C47">
+        <v>15.967542999999999</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>2.2227809999999995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <f>AVERAGE(D38:D47)</f>
+        <v>2.3266127000000005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <f>_xlfn.VAR.S(D38:D47)</f>
+        <v>1.3633726113344581E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>12.922606999999999</v>
+      </c>
+      <c r="C50">
+        <v>14.986534000000001</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>2.0639270000000014</v>
+      </c>
+      <c r="E50" s="3">
+        <v>8.8575618509102796E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>48.481748000000003</v>
+      </c>
+      <c r="C51">
+        <v>50.470053999999998</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>1.9883059999999944</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>48.148932000000002</v>
+      </c>
+      <c r="C52">
+        <v>50.291130000000003</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>2.1421980000000005</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>6.9148459999999998</v>
+      </c>
+      <c r="C53">
+        <v>8.8376669999999997</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>1.9228209999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>29.794836</v>
+      </c>
+      <c r="C54">
+        <v>31.905211000000001</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>2.1103750000000012</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>47.129576</v>
+      </c>
+      <c r="C55">
+        <v>49.038018000000001</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>1.9084420000000009</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>1.330095</v>
+      </c>
+      <c r="C56">
+        <v>3.2484229999999998</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>1.9183279999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>37.222330999999997</v>
+      </c>
+      <c r="C57">
+        <v>39.304017000000002</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>2.0816860000000048</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>52.401307000000003</v>
+      </c>
+      <c r="C58">
+        <v>54.605496000000002</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>2.2041889999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>13.329046999999999</v>
+      </c>
+      <c r="C59">
+        <v>15.242122</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>1.913075000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <f>AVERAGE(D50:D59)</f>
+        <v>2.0253347000000006</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <f>_xlfn.VAR.S(D50:D59)</f>
+        <v>1.1904371053788984E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>4</v>
+      </c>
+      <c r="B62">
+        <v>31.295694000000001</v>
+      </c>
+      <c r="C62">
+        <v>32.895746000000003</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ref="D62:D71" si="3">C62-B62</f>
+        <v>1.6000520000000016</v>
+      </c>
+      <c r="E62" s="3">
+        <v>9.4963317623950206E-3</v>
+      </c>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>55.312175000000003</v>
+      </c>
+      <c r="C63">
+        <v>57.164628999999998</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="3"/>
+        <v>1.8524539999999945</v>
+      </c>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>9.9465070000000004</v>
+      </c>
+      <c r="C64">
+        <v>11.56184</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="3"/>
+        <v>1.6153329999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>22.345037999999999</v>
+      </c>
+      <c r="C65">
+        <v>23.953841000000001</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="3"/>
+        <v>1.6088030000000018</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>43.033985000000001</v>
+      </c>
+      <c r="C66">
+        <v>44.839919000000002</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="3"/>
+        <v>1.8059340000000006</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>4.431489</v>
+      </c>
+      <c r="C67">
+        <v>6.0609010000000003</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="3"/>
+        <v>1.6294120000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>17.468677</v>
+      </c>
+      <c r="C68">
+        <v>19.227357000000001</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="3"/>
+        <v>1.7586800000000018</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>55.00018</v>
+      </c>
+      <c r="C69">
+        <v>56.610652999999999</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="3"/>
+        <v>1.6104729999999989</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>9.2591889999999992</v>
+      </c>
+      <c r="C70">
+        <v>10.980395</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="3"/>
+        <v>1.7212060000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>41.664808999999998</v>
+      </c>
+      <c r="C71">
+        <v>43.424627999999998</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="3"/>
+        <v>1.7598190000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <f>AVERAGE(D62:D71)</f>
+        <v>1.6962166000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <f>_xlfn.VAR.S(D62:D71)</f>
+        <v>8.9183543098220307E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>